<commit_message>
NL: -updated DESCRIPTION and NAMESPACE - added support to keeping and dropping columns while reading from a worksheet/named region - added getBoundingBox method - small change to clearNamedRegion unit tests
git-svn-id: svn://ms72.weblink.ch/mirai/XLConnect-R@277 ccc6e944-403e-a54a-b5f3-c2babcd103ea
</commit_message>
<xml_diff>
--- a/inst/unitTests/resources/testWorkbookClearCells.xlsx
+++ b/inst/unitTests/resources/testWorkbookClearCells.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="13395" windowHeight="6465" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="13395" windowHeight="6465" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="clearSheet1" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
   <definedNames>
     <definedName name="region1">clearNamedRegion!$B$2:$H$7</definedName>
     <definedName name="region2">clearNamedRegion!$F$10:$L$15</definedName>
+    <definedName name="region3">clearNamedRegion!$C$18:$I$23</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="7">
   <si>
     <t>one</t>
   </si>
@@ -43,9 +44,6 @@
   </si>
   <si>
     <t>seven</t>
-  </si>
-  <si>
-    <t>eight</t>
   </si>
 </sst>
 </file>
@@ -690,15 +688,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M15"/>
+  <dimension ref="B2:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10:M15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -720,11 +718,8 @@
       <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -746,11 +741,8 @@
       <c r="H3">
         <v>31</v>
       </c>
-      <c r="I3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
@@ -772,11 +764,8 @@
       <c r="H4">
         <v>32</v>
       </c>
-      <c r="I4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -798,11 +787,8 @@
       <c r="H5">
         <v>33</v>
       </c>
-      <c r="I5">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -824,11 +810,8 @@
       <c r="H6">
         <v>34</v>
       </c>
-      <c r="I6">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
@@ -850,11 +833,8 @@
       <c r="H7">
         <v>35</v>
       </c>
-      <c r="I7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>0</v>
       </c>
@@ -876,11 +856,8 @@
       <c r="L10" t="s">
         <v>6</v>
       </c>
-      <c r="M10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F11">
         <v>1</v>
       </c>
@@ -902,11 +879,8 @@
       <c r="L11">
         <v>31</v>
       </c>
-      <c r="M11">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F12">
         <v>2</v>
       </c>
@@ -928,11 +902,8 @@
       <c r="L12">
         <v>32</v>
       </c>
-      <c r="M12">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F13">
         <v>3</v>
       </c>
@@ -954,11 +925,8 @@
       <c r="L13">
         <v>33</v>
       </c>
-      <c r="M13">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F14">
         <v>4</v>
       </c>
@@ -980,11 +948,8 @@
       <c r="L14">
         <v>34</v>
       </c>
-      <c r="M14">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>5</v>
       </c>
@@ -1006,8 +971,143 @@
       <c r="L15">
         <v>35</v>
       </c>
-      <c r="M15">
-        <v>40</v>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>16</v>
+      </c>
+      <c r="G19">
+        <v>21</v>
+      </c>
+      <c r="H19">
+        <v>26</v>
+      </c>
+      <c r="I19">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>17</v>
+      </c>
+      <c r="G20">
+        <v>22</v>
+      </c>
+      <c r="H20">
+        <v>27</v>
+      </c>
+      <c r="I20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>13</v>
+      </c>
+      <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="G21">
+        <v>23</v>
+      </c>
+      <c r="H21">
+        <v>28</v>
+      </c>
+      <c r="I21">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>14</v>
+      </c>
+      <c r="F22">
+        <v>19</v>
+      </c>
+      <c r="G22">
+        <v>24</v>
+      </c>
+      <c r="H22">
+        <v>29</v>
+      </c>
+      <c r="I22">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+      <c r="F23">
+        <v>20</v>
+      </c>
+      <c r="G23">
+        <v>25</v>
+      </c>
+      <c r="H23">
+        <v>30</v>
+      </c>
+      <c r="I23">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1020,7 +1120,7 @@
   <dimension ref="C3:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:H7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>